<commit_message>
added extent html report utils and screenshot script
</commit_message>
<xml_diff>
--- a/testData/OrangeHRM_TestData.xlsx
+++ b/testData/OrangeHRM_TestData.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -469,7 +469,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
update test data for DDT
</commit_message>
<xml_diff>
--- a/testData/OrangeHRM_TestData.xlsx
+++ b/testData/OrangeHRM_TestData.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -469,7 +469,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>4</v>

</xml_diff>